<commit_message>
matin du 10e jour
</commit_message>
<xml_diff>
--- a/doc/Planning.xlsx
+++ b/doc/Planning.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
   <si>
     <t>TITRE DU PROJET</t>
   </si>
@@ -1852,22 +1852,36 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="36" fillId="18" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="36" fillId="18" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1900,492 +1914,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2869,8 +2397,8 @@
   </sheetPr>
   <dimension ref="A1:CA85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BR61" sqref="BR61:BT61"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BI70" sqref="BI70:BK70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -3548,7 +3076,7 @@
       <c r="BW8" s="138"/>
       <c r="BX8" s="138"/>
       <c r="BY8" s="138"/>
-      <c r="BZ8" s="186"/>
+      <c r="BZ8" s="189"/>
       <c r="CA8" s="23"/>
     </row>
     <row r="9" spans="1:79" ht="17.25" customHeight="1">
@@ -3667,7 +3195,7 @@
       </c>
       <c r="F10" s="27">
         <f>SUM(F11,F20,F27,F64,F73)</f>
-        <v>2.3611111111111107</v>
+        <v>2.65625</v>
       </c>
       <c r="G10" s="120">
         <v>45782</v>
@@ -5234,7 +4762,7 @@
       </c>
       <c r="F27" s="48">
         <f>SUM(F49:F56,F58:F63,F29:F40,F42:F47,)</f>
-        <v>1.3541666666666663</v>
+        <v>1.4374999999999998</v>
       </c>
       <c r="G27" s="49"/>
       <c r="H27" s="47"/>
@@ -7653,11 +7181,11 @@
       <c r="AT54" s="78"/>
       <c r="AU54" s="79"/>
       <c r="AV54" s="80"/>
-      <c r="AW54" s="187">
+      <c r="AW54" s="185">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="AX54" s="188"/>
-      <c r="AY54" s="189"/>
+      <c r="AX54" s="186"/>
+      <c r="AY54" s="187"/>
       <c r="AZ54" s="81"/>
       <c r="BA54" s="79"/>
       <c r="BB54" s="80"/>
@@ -8139,7 +7667,7 @@
       </c>
       <c r="F60" s="97">
         <f t="shared" ref="F60" si="36">SUM(G61:BZ61,)</f>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G60" s="87"/>
       <c r="H60" s="88"/>
@@ -8272,7 +7800,9 @@
       <c r="AZ61" s="81"/>
       <c r="BA61" s="79"/>
       <c r="BB61" s="80"/>
-      <c r="BC61" s="87"/>
+      <c r="BC61" s="87">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="BD61" s="88"/>
       <c r="BE61" s="89"/>
       <c r="BF61" s="78"/>
@@ -8489,7 +8019,7 @@
       </c>
       <c r="F64" s="32">
         <f>SUM(F65:F72)</f>
-        <v>0.52083333333333337</v>
+        <v>0.71875</v>
       </c>
       <c r="G64" s="63"/>
       <c r="H64" s="64"/>
@@ -8580,7 +8110,7 @@
       </c>
       <c r="F65" s="97">
         <f>SUM(G66:BZ66,)</f>
-        <v>0.25694444444444448</v>
+        <v>0.39236111111111116</v>
       </c>
       <c r="G65" s="87"/>
       <c r="H65" s="88"/>
@@ -8717,10 +8247,14 @@
       <c r="AZ66" s="81"/>
       <c r="BA66" s="79"/>
       <c r="BB66" s="80"/>
-      <c r="BC66" s="87"/>
+      <c r="BC66" s="87">
+        <v>5.9027777777777783E-2</v>
+      </c>
       <c r="BD66" s="88"/>
       <c r="BE66" s="89"/>
-      <c r="BF66" s="126"/>
+      <c r="BF66" s="126">
+        <v>7.6388888888888895E-2</v>
+      </c>
       <c r="BG66" s="79"/>
       <c r="BH66" s="80"/>
       <c r="BI66" s="169"/>
@@ -8758,7 +8292,7 @@
       </c>
       <c r="F67" s="97">
         <f t="shared" ref="F67" si="40">SUM(G68:BZ68,)</f>
-        <v>9.375E-2</v>
+        <v>0.15625</v>
       </c>
       <c r="G67" s="87"/>
       <c r="H67" s="88"/>
@@ -8942,7 +8476,9 @@
       <c r="BC68" s="87"/>
       <c r="BD68" s="88"/>
       <c r="BE68" s="89"/>
-      <c r="BF68" s="78"/>
+      <c r="BF68" s="78">
+        <v>6.25E-2</v>
+      </c>
       <c r="BG68" s="79"/>
       <c r="BH68" s="80"/>
       <c r="BI68" s="81"/>
@@ -9288,7 +8824,9 @@
       </c>
       <c r="AX72" s="79"/>
       <c r="AY72" s="80"/>
-      <c r="AZ72" s="81"/>
+      <c r="AZ72" s="81" t="s">
+        <v>91</v>
+      </c>
       <c r="BA72" s="79"/>
       <c r="BB72" s="80"/>
       <c r="BC72" s="87"/>
@@ -9332,7 +8870,7 @@
       </c>
       <c r="F73" s="42">
         <f t="shared" si="45"/>
-        <v>0.27430555555555558</v>
+        <v>0.28819444444444442</v>
       </c>
       <c r="G73" s="68"/>
       <c r="H73" s="69"/>
@@ -9423,7 +8961,7 @@
       </c>
       <c r="F74" s="97">
         <f>SUM(G75:BZ75)</f>
-        <v>0.11458333333333336</v>
+        <v>0.12847222222222224</v>
       </c>
       <c r="G74" s="110">
         <v>1.0416666666666666E-2</v>
@@ -9634,10 +9172,14 @@
       </c>
       <c r="BA75" s="150"/>
       <c r="BB75" s="151"/>
-      <c r="BC75" s="87"/>
+      <c r="BC75" s="87">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="BD75" s="90"/>
       <c r="BE75" s="152"/>
-      <c r="BF75" s="153"/>
+      <c r="BF75" s="153">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="BG75" s="90"/>
       <c r="BH75" s="152"/>
       <c r="BI75" s="149"/>
@@ -10027,7 +9569,7 @@
       <c r="BO79" s="78"/>
       <c r="BP79" s="79"/>
       <c r="BQ79" s="80"/>
-      <c r="BR79" s="185"/>
+      <c r="BR79" s="188"/>
       <c r="BS79" s="76"/>
       <c r="BT79" s="76"/>
       <c r="BU79" s="81"/>
@@ -10469,7 +10011,7 @@
       <c r="BB84" s="181"/>
       <c r="BC84" s="179">
         <f t="shared" ref="BC84" si="61">SUM(BC83:BH83,BC81:BH81,BC79:BH79,BC77:BH77,BC75:BH75,BC70:BH70,BC68:BH68,BC66:BH66,BC63:BH63,BC61:BH61,BC59:BH59,BC56:BH56,BC54:BH54,BC52:BH52,BC50:BH50,BC32:BH32,BC30:BH30,BC26:BH26,BC24:BH24,BC22:BH22,BC19:BH19,BC17:BH17,BC15:BH15,BC13:BH13,BC72:BH72,BC34:BH34,BC36:BH36,BC38:BH38,BC40:BH40,BC43:BH43,BC45:BH45,BC47:BH47,)</f>
-        <v>0</v>
+        <v>0.2951388888888889</v>
       </c>
       <c r="BD84" s="180"/>
       <c r="BE84" s="180"/>
@@ -12367,93 +11909,103 @@
     <mergeCell ref="BC72:BE72"/>
   </mergeCells>
   <conditionalFormatting sqref="G13:AV13 BF13:BZ13 G15:AV15 BF15:BZ15 G17:AV17 BF17:BZ17 G19:AV19 BF19:BZ19 G22:AV22 BF22:BZ22 G24:AV24 BF24:BZ24 G26:AV26 BF26:BZ26 G30:AV30 BF30:BZ30 G32:AV32 BF32:BZ32 G50:AV50 BF50:BZ50 G52:AV52 BF52:BZ52 G54:AV54 BF54:BZ54 G56:AV56 BF56:BZ56 G59:AV59 BF59:BZ59 G61:AV61 BF61:BZ61 G63:AV63 BF63:BZ63 G66:AV66 BF66 BI66:BZ66 G68:AV68 BF68:BZ68 G70:AV70 BF70:BZ70 G75:AV75 G77:AV77 BF77:BZ77 G79:AV79 BF79:BZ79 G81:AV81 BF81:BZ81 G83:AV83 BF83:BZ83">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="98">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="100">
       <formula>LEN(TRIM(G13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25:U25">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="64">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="66">
       <formula>LEN(TRIM(P25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC75:BE75 BC77:BE77 BC79:BE79 BC81:BE81 BC83:BE83">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="29">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="31">
       <formula>LEN(TRIM(BC75))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:AV34 BF34:BZ34">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="27">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="29">
       <formula>LEN(TRIM(G34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF75:BZ75">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="30">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="32">
       <formula>LEN(TRIM(BF75))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:AV36 BF36:BZ36">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="27">
       <formula>LEN(TRIM(G36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38:AV38 BF38:BZ38">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="25">
       <formula>LEN(TRIM(G38))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40:AV40 BF40:BZ40">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="23">
       <formula>LEN(TRIM(G40))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:AV43 BF43:BZ43">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="21">
       <formula>LEN(TRIM(G43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45:AV45 BF45:BZ45">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="18">
       <formula>LEN(TRIM(G45))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47:AV47 BF47:BZ47">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="15">
       <formula>LEN(TRIM(G47))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G72:AV72 BF72:BZ72">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="12">
       <formula>LEN(TRIM(G72))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT62:AV62 AT60:AV60 AT58:AV58 AQ55:AS55 AH49:AJ49 V39:X39 V37:X37 S35:X35 S33:U33">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="10">
       <formula>LEN(TRIM(S33))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK58:AP58">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(AK58))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW75:AY75">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(AW75))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW68:BB68">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(AW68))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW72:BB72 AW70:BB70 AW63:BB63 AW61:BB61 AW59:BB59 AW56:BB56">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(AW56))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ75:BB75">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(AZ75))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC61:BE61">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(BC61))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC66:BZ66">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(AZ75))&gt;0</formula>
+      <formula>LEN(TRIM(BC66))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>